<commit_message>
updated L5 desc and size and C4, C5 package size
</commit_message>
<xml_diff>
--- a/bill-of-materials/photon-bom-v010.xlsx
+++ b/bill-of-materials/photon-bom-v010.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\photon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\photon\bill-of-materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="157">
   <si>
     <t>SPARK SKU</t>
   </si>
@@ -496,6 +496,12 @@
   </si>
   <si>
     <t>100pF, Ceramic, 10V, 10%, X5R</t>
+  </si>
+  <si>
+    <t>2.2uH, 1.5A</t>
+  </si>
+  <si>
+    <t>3mm x 3mm</t>
   </si>
 </sst>
 </file>
@@ -644,7 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -685,6 +691,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1027,7 +1036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1153,8 +1164,8 @@
       <c r="D7" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
+      <c r="E7" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>19</v>
@@ -1415,10 +1426,10 @@
         <v>66</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>67</v>
+        <v>155</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>68</v>
+        <v>156</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>69</v>

</xml_diff>